<commit_message>
Update Angular Core 05 - Forms - DucDV7 Checklist.xlsx
</commit_message>
<xml_diff>
--- a/Angular Core 05 - Forms - DucDV7 Checklist.xlsx
+++ b/Angular Core 05 - Forms - DucDV7 Checklist.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/somallg/Desktop/FHO.FA.NEW/Reviewing/Front Ends/Angular 6/Angular Core 05 - Forms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EC.Angular01\EC_Angular_Checklist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570BD89E-8FDD-BB4E-A659-D8012C84639A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9540" yWindow="460" windowWidth="19260" windowHeight="16240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9540" yWindow="465" windowWidth="19260" windowHeight="16245" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Trainee</t>
   </si>
@@ -122,12 +121,26 @@
   </si>
   <si>
     <t>https://sitepoint-editors.github.io/account-registration-form/</t>
+  </si>
+  <si>
+    <t>Forms là thành phần đặc biệt trong trang web, chúng ta sử dụng form để thu nhập dữ liệu thông tin từ người dùng.</t>
+  </si>
+  <si>
+    <t>Có hai loại form trong Angular 4 là Templete Driven Form và Model Driven Form.
+Với temlate driven form thì phần lớn các công việc được thực hiện ở phía template và với model driven form (hay reactive form) thì công việc được thực hiện phần lớn ở component class.</t>
+  </si>
+  <si>
+    <t>Template dirven forms là phương pháp mà chúng ta sẽ tạo forms dựa vào template, chúng ta thực hiện việc thêm các directive và hành vi vào template, sau đó angular sẽ tự động tạo forms để quản lý và sử dụng.</t>
+  </si>
+  <si>
+    <t>Reactive forms hay còn gọi là model-driven forms, là phương pháp để tạo form trong angular, phương pháp này tránh việc sử dụng các directive ví dụ như ngModel,...
+Thay vào đó ta tạo các Object Model ở trong các component, rồi tạo form từ chúng.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -241,23 +254,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -599,503 +612,509 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-    </row>
-    <row r="26" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="C26" s="14" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+    </row>
+    <row r="26" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="C26" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-    </row>
-    <row r="27" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+    </row>
+    <row r="27" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E29" s="15" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E29" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E30" s="15" t="s">
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E30" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E31" s="15" t="s">
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E31" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E32" s="15" t="s">
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E32" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-    </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E33" s="15" t="s">
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+    </row>
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E33" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-    </row>
-    <row r="34" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E34" s="15" t="s">
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+    </row>
+    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E34" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-    </row>
-    <row r="35" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E35" s="15" t="s">
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+    </row>
+    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E35" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:N24"/>
+    <mergeCell ref="C26:L26"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E27:J27"/>
     <mergeCell ref="E34:G34"/>
     <mergeCell ref="E35:G35"/>
     <mergeCell ref="H29:J29"/>
@@ -1107,12 +1126,6 @@
     <mergeCell ref="E32:G32"/>
     <mergeCell ref="E33:G33"/>
     <mergeCell ref="H33:J33"/>
-    <mergeCell ref="A1:N24"/>
-    <mergeCell ref="C26:L26"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E27:J27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1121,30 +1134,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="62.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" customWidth="1"/>
+    <col min="6" max="6" width="106" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" s="9"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1161,7 +1175,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1177,8 +1191,11 @@
       <c r="E5" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1189,8 +1206,11 @@
       <c r="D6" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1205,7 +1225,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1217,8 +1237,11 @@
         <v>6</v>
       </c>
       <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1231,7 +1254,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1248,7 +1271,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1259,8 +1282,11 @@
       <c r="D11" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1275,7 +1301,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1300,14 +1326,14 @@
     <mergeCell ref="B10:B12"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:D1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:D1048576">
       <formula1>"YES, NO"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E10" r:id="rId1" xr:uid="{57EB0AA8-9676-A64D-B521-00850E04B1EB}"/>
-    <hyperlink ref="E13" r:id="rId2" xr:uid="{659E14E2-F680-1D4D-999C-0E5801D97B05}"/>
-    <hyperlink ref="E12" r:id="rId3" xr:uid="{6255464A-EDBD-F442-9A50-B5421CB638CA}"/>
+    <hyperlink ref="E10" r:id="rId1"/>
+    <hyperlink ref="E13" r:id="rId2"/>
+    <hyperlink ref="E12" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>

</xml_diff>